<commit_message>
new commit on dec 19th 2020
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/LoginKeywords.xlsx
+++ b/src/test/resources/testdata/LoginKeywords.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="18090" windowHeight="5700"/>
+    <workbookView xWindow="0" yWindow="2850" windowWidth="18090" windowHeight="5700"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -551,7 +551,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>